<commit_message>
updated picklists and table schema for DC 2021
</commit_message>
<xml_diff>
--- a/config/PredefinedResults.xlsx
+++ b/config/PredefinedResults.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eclipse_workspace\tse_workspace\tse-data-reporting-tool\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eclipse_workspace\tse_workspace\tse-reporting-tool\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CA7480-EB0C-41CD-8AEA-40EEEA9CB16D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75337BD-0B51-4417-A074-5848FF4C28B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="144">
   <si>
     <t>sampAnAsses</t>
   </si>
@@ -473,6 +473,9 @@
   </si>
   <si>
     <t>Goat</t>
+  </si>
+  <si>
+    <t>AT11A - Discriminatory</t>
   </si>
 </sst>
 </file>
@@ -1715,7 +1718,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G28" sqref="G28:G29"/>
@@ -2969,8 +2972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3739,11 +3742,11 @@
         <v>19</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>28</v>
+        <v>143</v>
       </c>
       <c r="C26" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
-        <v>CWDAT12A</v>
+        <v>CWDAT11A</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>30</v>
@@ -3769,11 +3772,11 @@
         <v>19</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>28</v>
+        <v>143</v>
       </c>
       <c r="C27" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
-        <v>CWDAT12A</v>
+        <v>CWDAT11A</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>19</v>
@@ -3799,11 +3802,11 @@
         <v>19</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>28</v>
+        <v>143</v>
       </c>
       <c r="C28" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
-        <v>CWDAT12A</v>
+        <v>CWDAT11A</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>45</v>
@@ -3829,11 +3832,11 @@
         <v>19</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>28</v>
+        <v>143</v>
       </c>
       <c r="C29" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
-        <v>CWDAT12A</v>
+        <v>CWDAT11A</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
changed predefinedResults, picklists and other ui optimisations
</commit_message>
<xml_diff>
--- a/config/PredefinedResults.xlsx
+++ b/config/PredefinedResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eclipse_workspace\tse_workspace\tse-reporting-tool\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75337BD-0B51-4417-A074-5848FF4C28B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D66FE8-A7C4-499D-9A7B-A754C602689F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17880" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,10 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="144">
-  <si>
-    <t>sampAnAsses</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="145">
   <si>
     <t>recordType</t>
   </si>
@@ -109,9 +106,6 @@
     <t>J049A</t>
   </si>
   <si>
-    <t>BSE-not excluded</t>
-  </si>
-  <si>
     <t>Classical-scrapie</t>
   </si>
   <si>
@@ -415,9 +409,6 @@
     <t>genotypingBaseTerm</t>
   </si>
   <si>
-    <t>sampAnAssesLabel</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -451,12 +442,6 @@
     <t>RF-00004898-PAR$POS</t>
   </si>
   <si>
-    <t>RGT</t>
-  </si>
-  <si>
-    <t>RF-00004629-PAR</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
@@ -476,6 +461,24 @@
   </si>
   <si>
     <t>AT11A - Discriminatory</t>
+  </si>
+  <si>
+    <t>sampEventAsses</t>
+  </si>
+  <si>
+    <t>sampEventAssesLabel</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>BSE-not excluded (i.e. BSE like)</t>
+  </si>
+  <si>
+    <t>Classical-scrapie (i.e. BSE-excluded in 1st Molecular test)</t>
+  </si>
+  <si>
+    <t>J054A</t>
   </si>
 </sst>
 </file>
@@ -508,7 +511,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -527,7 +529,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -588,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -598,13 +600,23 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,7 +665,7 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -673,7 +685,13 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="thin">
@@ -682,8 +700,6 @@
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -702,7 +718,13 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="thin">
@@ -711,8 +733,6 @@
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -734,7 +754,7 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -1356,15 +1376,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J45" totalsRowShown="0" dataDxfId="24">
-  <autoFilter ref="A1:J45" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J51" totalsRowShown="0" dataDxfId="24">
+  <autoFilter ref="A1:J51" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J51">
+    <sortCondition ref="A2:A51"/>
+    <sortCondition ref="B2:B51"/>
+    <sortCondition descending="1" ref="D2:D51"/>
+    <sortCondition ref="E2:E51"/>
+  </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="recordType" dataDxfId="23"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="source" dataDxfId="22"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="sourceLabel" dataDxfId="21"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="confirmatoryExecuted" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="sampAnAsses" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="sampAnAssesLabel" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="sampEventAsses" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="sampEventAssesLabel" dataDxfId="18"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="screening" dataDxfId="17"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="confirmatory" dataDxfId="16"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="discriminatory" dataDxfId="15"/>
@@ -1715,20 +1741,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G28" sqref="G28:G29"/>
+      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.6640625" customWidth="1"/>
     <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="3" max="3" width="6.21875" customWidth="1"/>
     <col min="4" max="4" width="5.21875" customWidth="1"/>
     <col min="5" max="5" width="8.33203125" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
@@ -1740,1225 +1766,1389 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>123</v>
-      </c>
       <c r="G1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="G2" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>106</v>
       </c>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
+        <v>121</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H3" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="I3" s="19" t="s">
         <v>105</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>121</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>106</v>
       </c>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>132</v>
+        <v>103</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="H6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="J7" s="1"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G8" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="15" t="s">
-        <v>108</v>
       </c>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="E9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G9" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9" s="8" t="s">
-        <v>107</v>
+      <c r="I9" s="19" t="s">
+        <v>105</v>
       </c>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>3</v>
+        <v>122</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>8</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10" s="15" t="s">
-        <v>132</v>
+      <c r="I10" s="18" t="s">
+        <v>106</v>
       </c>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H11" s="2"/>
-      <c r="I11" s="15" t="s">
-        <v>103</v>
+      <c r="I11" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="F13" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="I12" s="8"/>
-      <c r="J12" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="G13" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H13" s="12"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>141</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
       <c r="D14" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>120</v>
+        <v>15</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>142</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>96</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>141</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
       <c r="D15" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>94</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>141</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
       <c r="D16" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>97</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I17" s="9"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="F18" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H17" s="1" t="s">
+      <c r="G18" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="H18" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="I18" s="8"/>
-      <c r="J18" s="1"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>118</v>
-      </c>
       <c r="G19" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="I19" s="8" t="s">
         <v>112</v>
+      </c>
+      <c r="H19" s="9"/>
+      <c r="I19" s="19" t="s">
+        <v>114</v>
       </c>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>142</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="D20" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>119</v>
+        <v>19</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>120</v>
+        <v>18</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="I20" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="H20" s="9"/>
+      <c r="I20" s="19" t="s">
         <v>113</v>
       </c>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>142</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E21" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F21" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="G21" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="I21" s="15" t="s">
-        <v>111</v>
+        <v>112</v>
+      </c>
+      <c r="H21" s="18"/>
+      <c r="I21" s="8" t="s">
+        <v>131</v>
       </c>
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>142</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
       <c r="D22" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>3</v>
       </c>
       <c r="F22" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="H22" s="21"/>
+      <c r="I22" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="J22" s="8"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="16"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="E24" s="8" t="s">
+      <c r="F24" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="8" t="s">
-        <v>15</v>
-      </c>
       <c r="G24" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="8" t="s">
-        <v>110</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="I24" s="19"/>
       <c r="J24" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>118</v>
+        <v>15</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>142</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H25" s="1"/>
-      <c r="I25" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>95</v>
+        <v>107</v>
+      </c>
+      <c r="H25" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="I25" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="J25" s="21" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>120</v>
+        <v>16</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>143</v>
       </c>
       <c r="G26" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H26" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="I26" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="H26" s="15"/>
-      <c r="I26" s="8" t="s">
-        <v>113</v>
-      </c>
       <c r="J26" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>22</v>
+        <v>2</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>94</v>
+        <v>107</v>
+      </c>
+      <c r="H27" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="I27" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="J27" s="19" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>3</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H28" s="15"/>
-      <c r="I28" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>97</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I28" s="21"/>
+      <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H29" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="I29" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="F30" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H29" s="8"/>
-      <c r="I29" s="15" t="s">
+      <c r="G30" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H30" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H30" s="1"/>
-      <c r="I30" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="J30" s="1"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="13"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E31" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>16</v>
-      </c>
       <c r="F31" s="8" t="s">
-        <v>118</v>
+        <v>14</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H31" s="1"/>
-      <c r="I31" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="J31" s="1"/>
+      <c r="I31" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>119</v>
+        <v>15</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H32" s="15"/>
-      <c r="I32" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="J32" s="1"/>
+        <v>107</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="J32" s="21" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G33" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H33" s="18"/>
+      <c r="I33" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="J33" s="1"/>
+      <c r="J33" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H34" s="15"/>
-      <c r="I34" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="J34" s="8"/>
+        <v>107</v>
+      </c>
+      <c r="H34" s="9"/>
+      <c r="I34" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="J34" s="19" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15" t="s">
-        <v>103</v>
+        <v>11</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="H35" s="19"/>
+      <c r="I35" s="18" t="s">
+        <v>101</v>
       </c>
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="D36" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>20</v>
+        <v>117</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="H36" s="8" t="s">
-        <v>105</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="H36" s="9"/>
       <c r="I36" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="J36" s="1"/>
+        <v>111</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="H37" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="J37" s="1"/>
+      <c r="A37" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E37" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="F37" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G37" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="H37" s="13"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="13"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="D38" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="H38" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="I38" s="8" t="s">
-        <v>134</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="H38" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="I38" s="19"/>
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="D39" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>142</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="H39" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H39" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="I39" s="15"/>
-      <c r="J39" s="1"/>
+      <c r="I39" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="J39" s="21"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="D40" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>143</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="H40" s="15"/>
-      <c r="I40" s="8" t="s">
-        <v>115</v>
+        <v>107</v>
+      </c>
+      <c r="H40" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="D41" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>118</v>
+        <v>2</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="H41" s="15"/>
-      <c r="I41" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="J41" s="1"/>
+        <v>107</v>
+      </c>
+      <c r="H41" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="I41" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="J41" s="19"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="D42" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>3</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G42" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="H42" s="15"/>
-      <c r="I42" s="8" t="s">
-        <v>134</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="H42" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="I42" s="21"/>
       <c r="J42" s="1"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="D43" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>12</v>
+        <v>118</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="H43" s="7"/>
+        <v>107</v>
+      </c>
+      <c r="H43" s="24" t="s">
+        <v>103</v>
+      </c>
       <c r="I43" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="J43" s="7"/>
+        <v>111</v>
+      </c>
+      <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="13" t="s">
-        <v>136</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H44" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="I44" s="15"/>
+      <c r="J44" s="13"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="13"/>
+        <v>12</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H45" s="15"/>
       <c r="I45" s="13"/>
-      <c r="J45" s="13" t="s">
-        <v>136</v>
-      </c>
+      <c r="J45" s="13"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H46" s="21"/>
+      <c r="I46" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H47" s="1"/>
+      <c r="I47" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H48" s="9"/>
+      <c r="I48" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H49" s="9"/>
+      <c r="I49" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="J49" s="19"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="H50" s="22"/>
+      <c r="I50" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="J50" s="7"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E51" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F51" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="G51" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="H51" s="9"/>
+      <c r="I51" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="J51" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2972,8 +3162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:B29"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2990,871 +3180,871 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT06A</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>129</v>
-      </c>
       <c r="I2" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT06A</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT08A</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT08A</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT12A</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT12A</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>23</v>
+        <v>35</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT12A</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>23</v>
+        <v>36</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C9" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT12A</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>23</v>
+        <v>37</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT12A</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>132</v>
+        <v>49</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>129</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT06A</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="F11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>130</v>
-      </c>
       <c r="I11" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT06A</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT08A</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT08A</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>23</v>
+        <v>40</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT08A</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" t="s">
-        <v>93</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>23</v>
+        <v>39</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT12A</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C17" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT12A</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E17" t="s">
-        <v>93</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>23</v>
+      <c r="G17" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C18" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT12A</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" t="s">
-        <v>94</v>
+        <v>42</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>92</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>23</v>
+        <v>42</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C19" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT12A</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" t="s">
-        <v>95</v>
+        <v>43</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>93</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>23</v>
+        <v>50</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C20" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT12A</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>23</v>
+        <v>51</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C21" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT12A</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>133</v>
+        <v>45</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>130</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C22" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT06A</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="F22" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="G22" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>131</v>
-      </c>
       <c r="I22" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C23" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT06A</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>23</v>
+        <v>96</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C24" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT08A</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C25" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT08A</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C26" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT11A</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C27" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT11A</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>23</v>
+        <v>97</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C28" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT11A</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>23</v>
+        <v>98</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C29" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT11A</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>134</v>
+        <v>99</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>131</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3870,9 +4060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3882,130 +4070,130 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[4] Automatically create rows for tse(os) | sample -> result
</commit_message>
<xml_diff>
--- a/config/PredefinedResults.xlsx
+++ b/config/PredefinedResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eclipse_workspace\tse_workspace\tse-reporting-tool\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p70837\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F94FC8-0EFB-437A-BDBF-2EEE58484014}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08654C34-5F66-4588-83E1-C9FC55509348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="2895" windowWidth="28800" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="149">
   <si>
     <t>recordType</t>
   </si>
@@ -479,6 +479,18 @@
   </si>
   <si>
     <t>CWDAT11A_4</t>
+  </si>
+  <si>
+    <t>BSEOS</t>
+  </si>
+  <si>
+    <t>Positive (other tse)</t>
+  </si>
+  <si>
+    <t>Bse-not excluded (ie BSE like)</t>
+  </si>
+  <si>
+    <t>J055A</t>
   </si>
 </sst>
 </file>
@@ -590,37 +602,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1380,11 +1393,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J51" totalsRowShown="0" dataDxfId="24">
-  <autoFilter ref="A1:J51" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J61" totalsRowShown="0" dataDxfId="24">
+  <autoFilter ref="A1:J61" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="CWD"/>
+        <filter val="BSE"/>
+        <filter val="BSEOS"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1748,30 +1762,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F46" sqref="F46"/>
+      <selection pane="bottomRight" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
-    <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" customWidth="1"/>
-    <col min="8" max="8" width="24.44140625" customWidth="1"/>
-    <col min="9" max="9" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1784,10 +1798,10 @@
       <c r="D1" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="27" t="s">
         <v>136</v>
       </c>
       <c r="G1" t="s">
@@ -1803,7 +1817,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1813,27 +1827,27 @@
       <c r="C2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="I2" s="21"/>
+      <c r="I2" s="6"/>
       <c r="J2" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1843,27 +1857,27 @@
       <c r="C3" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="17" t="s">
+      <c r="H3" s="13"/>
+      <c r="I3" s="14" t="s">
         <v>104</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1873,27 +1887,27 @@
       <c r="C4" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="11" t="s">
+      <c r="I4" s="6"/>
+      <c r="J4" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1903,27 +1917,27 @@
       <c r="C5" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="17" t="s">
+      <c r="H5" s="13"/>
+      <c r="I5" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -1933,27 +1947,27 @@
       <c r="C6" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H6" s="29"/>
-      <c r="I6" s="17" t="s">
+      <c r="H6" s="19"/>
+      <c r="I6" s="14" t="s">
         <v>106</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1963,79 +1977,79 @@
       <c r="C7" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="14" t="s">
         <v>106</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>108</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="6" t="s">
         <v>110</v>
       </c>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H9" s="27"/>
-      <c r="I9" s="17" t="s">
+      <c r="H9" s="19"/>
+      <c r="I9" s="14" t="s">
         <v>110</v>
       </c>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -2045,27 +2059,27 @@
       <c r="C10" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H10" s="29"/>
-      <c r="I10" s="21" t="s">
+      <c r="H10" s="19"/>
+      <c r="I10" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2075,35 +2089,35 @@
       <c r="C11" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>103</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="J11" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>117</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -2112,24 +2126,24 @@
       <c r="F12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="6" t="s">
         <v>98</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="I12" s="14" t="s">
         <v>100</v>
       </c>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>118</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -2138,16 +2152,15 @@
       <c r="F13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="17" t="s">
+      <c r="I13" s="14" t="s">
         <v>100</v>
       </c>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -2157,27 +2170,27 @@
       <c r="C14" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16" t="s">
+      <c r="H14" s="13"/>
+      <c r="I14" s="13" t="s">
         <v>105</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2187,29 +2200,29 @@
       <c r="C15" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I15" s="16" t="s">
+      <c r="I15" s="13" t="s">
         <v>105</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -2219,27 +2232,27 @@
       <c r="C16" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16" t="s">
+      <c r="H16" s="13"/>
+      <c r="I16" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="J16" s="11" t="s">
+      <c r="J16" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -2249,29 +2262,29 @@
       <c r="C17" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H17" s="21" t="s">
+      <c r="H17" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J17" s="11" t="s">
+      <c r="J17" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
@@ -2281,27 +2294,27 @@
       <c r="C18" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H18" s="16"/>
-      <c r="I18" s="21" t="s">
+      <c r="H18" s="13"/>
+      <c r="I18" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="J18" s="21" t="s">
+      <c r="J18" s="6" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
@@ -2311,29 +2324,29 @@
       <c r="C19" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H19" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="I19" s="17" t="s">
+      <c r="I19" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="J19" s="17" t="s">
+      <c r="J19" s="14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
@@ -2343,27 +2356,27 @@
       <c r="C20" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H20" s="8"/>
-      <c r="I20" s="17" t="s">
+      <c r="H20" s="1"/>
+      <c r="I20" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="J20" s="20" t="s">
+      <c r="J20" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
@@ -2373,153 +2386,152 @@
       <c r="C21" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H21" s="21" t="s">
+      <c r="H21" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I21" s="21" t="s">
+      <c r="I21" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="J21" s="23" t="s">
+      <c r="J21" s="16" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="H22" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I22" s="7" t="s">
+      <c r="I22" s="6" t="s">
         <v>109</v>
       </c>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G23" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H23" s="16"/>
-      <c r="I23" s="21" t="s">
+      <c r="H23" s="13"/>
+      <c r="I23" s="6" t="s">
         <v>109</v>
       </c>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F24" s="19" t="s">
+      <c r="F24" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G24" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="H24" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I24" s="17" t="s">
+      <c r="I24" s="14" t="s">
         <v>101</v>
       </c>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="19" t="s">
+      <c r="F25" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="H25" s="26"/>
-      <c r="I25" s="21" t="s">
+      <c r="I25" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="J25" s="19"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J25" s="13"/>
+    </row>
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G26" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="17" t="s">
+      <c r="H26" s="1"/>
+      <c r="I26" s="14" t="s">
         <v>127</v>
       </c>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
@@ -2529,16 +2541,16 @@
       <c r="C27" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="7" t="s">
         <v>123</v>
       </c>
       <c r="H27" s="1" t="s">
@@ -2547,7 +2559,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>12</v>
       </c>
@@ -2557,101 +2569,101 @@
       <c r="C28" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="G28" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="H28" s="17"/>
-      <c r="I28" s="16" t="s">
+      <c r="H28" s="14"/>
+      <c r="I28" s="13" t="s">
         <v>97</v>
       </c>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="E29" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F29" s="19" t="s">
+      <c r="F29" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="G29" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="H29" s="17" t="s">
+      <c r="H29" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="I29" s="16" t="s">
+      <c r="I29" s="13" t="s">
         <v>125</v>
       </c>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E30" s="19" t="s">
+      <c r="E30" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F30" s="19" t="s">
+      <c r="F30" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="G30" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="H30" s="25"/>
-      <c r="I30" s="16" t="s">
+      <c r="H30" s="18"/>
+      <c r="I30" s="13" t="s">
         <v>125</v>
       </c>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G31" s="7" t="s">
+      <c r="G31" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H31" s="17" t="s">
+      <c r="H31" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="I31" s="17" t="s">
+      <c r="I31" s="14" t="s">
         <v>127</v>
       </c>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>12</v>
       </c>
@@ -2661,25 +2673,25 @@
       <c r="C32" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E32" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="F32" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="G32" s="7" t="s">
         <v>123</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-    </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+    </row>
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>12</v>
       </c>
@@ -2689,43 +2701,43 @@
       <c r="C33" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="F33" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G33" s="10" t="s">
+      <c r="G33" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="H33" s="16"/>
-      <c r="I33" s="8" t="s">
+      <c r="H33" s="13"/>
+      <c r="I33" s="1" t="s">
         <v>97</v>
       </c>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E34" s="13" t="s">
+      <c r="E34" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F34" s="19" t="s">
+      <c r="F34" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G34" s="7" t="s">
+      <c r="G34" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="H34" s="17" t="s">
+      <c r="H34" s="14" t="s">
         <v>99</v>
       </c>
       <c r="I34" s="1" t="s">
@@ -2733,127 +2745,127 @@
       </c>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E35" s="13" t="s">
+      <c r="E35" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="19" t="s">
+      <c r="F35" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="7" t="s">
+      <c r="G35" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="H35" s="25"/>
-      <c r="I35" s="16" t="s">
+      <c r="H35" s="18"/>
+      <c r="I35" s="13" t="s">
         <v>102</v>
       </c>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E36" s="19" t="s">
+      <c r="E36" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F36" s="19" t="s">
+      <c r="F36" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G36" s="10" t="s">
+      <c r="G36" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="H36" s="28" t="s">
+      <c r="H36" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="I36" s="16"/>
+      <c r="I36" s="13"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F37" s="19" t="s">
+      <c r="F37" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G37" s="7" t="s">
+      <c r="G37" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="H37" s="25"/>
-      <c r="I37" s="16" t="s">
+      <c r="H37" s="18"/>
+      <c r="I37" s="13" t="s">
         <v>97</v>
       </c>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E38" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F38" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G38" s="10" t="s">
+      <c r="G38" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="H38" s="17" t="s">
+      <c r="H38" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="I38" s="8"/>
+      <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="E39" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="F39" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G39" s="10" t="s">
+      <c r="G39" s="7" t="s">
         <v>124</v>
       </c>
       <c r="H39" s="1"/>
-      <c r="I39" s="7" t="s">
+      <c r="I39" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J39" s="19"/>
-    </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="J39" s="13"/>
+    </row>
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>12</v>
       </c>
@@ -2863,29 +2875,29 @@
       <c r="C40" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D40" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E40" s="21" t="s">
+      <c r="E40" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F40" s="21" t="s">
+      <c r="F40" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="G40" s="7" t="s">
+      <c r="G40" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H40" s="17" t="s">
+      <c r="H40" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="I40" s="17" t="s">
+      <c r="I40" s="14" t="s">
         <v>107</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>12</v>
       </c>
@@ -2895,27 +2907,27 @@
       <c r="C41" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E41" s="21" t="s">
+      <c r="E41" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F41" s="21" t="s">
+      <c r="F41" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="G41" s="7" t="s">
+      <c r="G41" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H41" s="8"/>
-      <c r="I41" s="17" t="s">
+      <c r="H41" s="1"/>
+      <c r="I41" s="14" t="s">
         <v>107</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>12</v>
       </c>
@@ -2925,29 +2937,29 @@
       <c r="C42" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F42" s="7" t="s">
+      <c r="F42" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="G42" s="7" t="s">
+      <c r="G42" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I42" s="7" t="s">
+      <c r="I42" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="J42" s="11" t="s">
+      <c r="J42" s="8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>12</v>
       </c>
@@ -2957,246 +2969,487 @@
       <c r="C43" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E43" s="21" t="s">
+      <c r="E43" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F43" s="21" t="s">
+      <c r="F43" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="G43" s="21" t="s">
+      <c r="G43" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H43" s="16"/>
-      <c r="I43" s="21" t="s">
+      <c r="H43" s="13"/>
+      <c r="I43" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="J43" s="11" t="s">
+      <c r="J43" s="8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="11" t="s">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="12" t="s">
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="E44" s="13" t="s">
+      <c r="E44" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="F44" s="13" t="s">
+      <c r="F44" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="G44" s="10" t="s">
+      <c r="G44" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="H44" s="10" t="s">
+      <c r="H44" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="I44" s="13"/>
-      <c r="J44" s="11"/>
-    </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="11" t="s">
+      <c r="I44" s="10"/>
+      <c r="J44" s="8"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="12" t="s">
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E45" s="13" t="s">
+      <c r="E45" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="F45" s="13" t="s">
+      <c r="F45" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="G45" s="10" t="s">
+      <c r="G45" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="H45" s="10"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="11" t="s">
+      <c r="H45" s="7"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+    </row>
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="12" t="s">
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="E46" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="F46" s="10" t="s">
+      <c r="F46" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="G46" s="10" t="s">
+      <c r="G46" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="H46" s="10" t="s">
+      <c r="H46" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="I46" s="13"/>
-      <c r="J46" s="11"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="11" t="s">
+      <c r="I46" s="10"/>
+      <c r="J46" s="8"/>
+    </row>
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="12" t="s">
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E47" s="13" t="s">
+      <c r="E47" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="F47" s="13" t="s">
+      <c r="F47" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="G47" s="15" t="s">
+      <c r="G47" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="H47" s="14"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="14"/>
-    </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="11" t="s">
+      <c r="H47" s="11"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="11"/>
+    </row>
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="D48" s="12" t="s">
+      <c r="D48" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="E48" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="F48" s="10" t="s">
+      <c r="F48" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="G48" s="10" t="s">
+      <c r="G48" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="H48" s="11" t="s">
+      <c r="H48" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="I48" s="23" t="s">
+      <c r="I48" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="J48" s="23" t="s">
+      <c r="J48" s="16" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="11" t="s">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D49" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E49" s="20" t="s">
+      <c r="E49" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="F49" s="20" t="s">
+      <c r="F49" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="G49" s="10" t="s">
+      <c r="G49" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="H49" s="13"/>
-      <c r="I49" s="20" t="s">
+      <c r="H49" s="10"/>
+      <c r="I49" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="J49" s="20" t="s">
+      <c r="J49" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="11" t="s">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="D50" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="E50" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="F50" s="10" t="s">
+      <c r="F50" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="G50" s="10" t="s">
+      <c r="G50" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="H50" s="24" t="s">
+      <c r="H50" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="I50" s="23" t="s">
+      <c r="I50" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="J50" s="23" t="s">
+      <c r="J50" s="16" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="11" t="s">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="D51" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E51" s="23" t="s">
+      <c r="E51" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="F51" s="23" t="s">
+      <c r="F51" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="G51" s="10" t="s">
+      <c r="G51" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="H51" s="13"/>
-      <c r="I51" s="20" t="s">
+      <c r="H51" s="10"/>
+      <c r="I51" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="J51" s="20" t="s">
+      <c r="J51" s="7" t="s">
         <v>91</v>
       </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="F52" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="G52" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="H52" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="I52" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="J52" s="21"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B53" s="23"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="E53" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="F53" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="G53" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="H53" s="30"/>
+      <c r="I53" s="30"/>
+      <c r="J53" s="23"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E54" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="G54" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="H54" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="I54" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E55" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="G55" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="H55" s="30"/>
+      <c r="I55" s="30"/>
+      <c r="J55" s="13"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F56" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H56" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="I56" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="J56" s="1"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F57" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H57" s="18"/>
+      <c r="I57" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="J57" s="1"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="H58" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="I58" s="13"/>
+      <c r="J58" s="1"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E59" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F59" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H59" s="18"/>
+      <c r="I59" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="J59" s="1"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H60" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="I60" s="10"/>
+      <c r="J60" s="8"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H61" s="7"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3205,23 +3458,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
-    <col min="4" max="4" width="28.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="27.44140625" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3250,7 +3503,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3261,26 +3514,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT06A</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -3291,26 +3544,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT06A</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -3321,26 +3574,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT08A</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -3351,26 +3604,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT08A</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -3381,26 +3634,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT12A</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -3411,26 +3664,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT12A</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -3441,26 +3694,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT12A</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -3471,26 +3724,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT12A</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -3501,26 +3754,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT12A</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -3531,26 +3784,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT06A</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -3561,26 +3814,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT06A</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -3591,26 +3844,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT08A</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="I13" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -3621,26 +3874,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT08A</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I14" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -3651,26 +3904,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT08A</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" t="s">
         <v>87</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -3681,26 +3934,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT12A</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="H16" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="I16" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -3711,26 +3964,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT12A</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" t="s">
         <v>87</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="I17" s="7" t="s">
+      <c r="I17" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -3744,23 +3997,23 @@
       <c r="D18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E18" t="s">
         <v>88</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="H18" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="I18" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
@@ -3774,23 +4027,23 @@
       <c r="D19" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" t="s">
         <v>89</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H19" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="I19" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
@@ -3810,17 +4063,17 @@
       <c r="F20" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="H20" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="I20" s="7" t="s">
+      <c r="I20" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
@@ -3840,17 +4093,17 @@
       <c r="F21" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="H21" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="I21" s="7" t="s">
+      <c r="I21" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>18</v>
       </c>
@@ -3861,26 +4114,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT06A</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="H22" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="I22" s="7" t="s">
+      <c r="I22" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>18</v>
       </c>
@@ -3891,26 +4144,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT06A</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="H23" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I23" s="7" t="s">
+      <c r="I23" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>18</v>
       </c>
@@ -3921,26 +4174,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT08A</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="H24" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="I24" s="7" t="s">
+      <c r="I24" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
@@ -3951,26 +4204,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT08A</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="G25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="H25" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I25" s="7" t="s">
+      <c r="I25" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>18</v>
       </c>
@@ -3981,26 +4234,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT11A</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H26" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="I26" s="7" t="s">
+      <c r="I26" s="6" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>18</v>
       </c>
@@ -4011,26 +4264,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT11A</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="G27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="H27" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="I27" s="7" t="s">
+      <c r="I27" s="6" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>18</v>
       </c>
@@ -4047,20 +4300,20 @@
       <c r="E28" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="G28" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H28" s="7" t="s">
+      <c r="H28" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="I28" s="7" t="s">
+      <c r="I28" s="6" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>18</v>
       </c>
@@ -4077,16 +4330,16 @@
       <c r="E29" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="G29" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H29" s="7" t="s">
+      <c r="H29" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="I29" s="7" t="s">
+      <c r="I29" s="6" t="s">
         <v>144</v>
       </c>
     </row>
@@ -4105,13 +4358,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -4119,7 +4372,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>81</v>
       </c>
@@ -4127,7 +4380,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -4135,7 +4388,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -4143,7 +4396,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -4151,7 +4404,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>85</v>
       </c>
@@ -4159,7 +4412,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>86</v>
       </c>
@@ -4167,7 +4420,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>87</v>
       </c>
@@ -4175,7 +4428,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>88</v>
       </c>
@@ -4183,7 +4436,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -4191,7 +4444,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -4199,7 +4452,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -4207,7 +4460,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>92</v>
       </c>
@@ -4215,7 +4468,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -4223,7 +4476,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -4231,7 +4484,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>95</v>
       </c>

</xml_diff>

<commit_message>
July 31st, 2023 changes (#2)
</commit_message>
<xml_diff>
--- a/config/PredefinedResults.xlsx
+++ b/config/PredefinedResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eclipse_workspace\tse_workspace\tse-reporting-tool\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p70837\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F94FC8-0EFB-437A-BDBF-2EEE58484014}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08654C34-5F66-4588-83E1-C9FC55509348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="2895" windowWidth="28800" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="149">
   <si>
     <t>recordType</t>
   </si>
@@ -479,6 +479,18 @@
   </si>
   <si>
     <t>CWDAT11A_4</t>
+  </si>
+  <si>
+    <t>BSEOS</t>
+  </si>
+  <si>
+    <t>Positive (other tse)</t>
+  </si>
+  <si>
+    <t>Bse-not excluded (ie BSE like)</t>
+  </si>
+  <si>
+    <t>J055A</t>
   </si>
 </sst>
 </file>
@@ -590,37 +602,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1380,11 +1393,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J51" totalsRowShown="0" dataDxfId="24">
-  <autoFilter ref="A1:J51" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J61" totalsRowShown="0" dataDxfId="24">
+  <autoFilter ref="A1:J61" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="CWD"/>
+        <filter val="BSE"/>
+        <filter val="BSEOS"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1748,30 +1762,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F46" sqref="F46"/>
+      <selection pane="bottomRight" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
-    <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" customWidth="1"/>
-    <col min="8" max="8" width="24.44140625" customWidth="1"/>
-    <col min="9" max="9" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1784,10 +1798,10 @@
       <c r="D1" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="27" t="s">
         <v>136</v>
       </c>
       <c r="G1" t="s">
@@ -1803,7 +1817,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1813,27 +1827,27 @@
       <c r="C2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="I2" s="21"/>
+      <c r="I2" s="6"/>
       <c r="J2" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1843,27 +1857,27 @@
       <c r="C3" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="17" t="s">
+      <c r="H3" s="13"/>
+      <c r="I3" s="14" t="s">
         <v>104</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1873,27 +1887,27 @@
       <c r="C4" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="11" t="s">
+      <c r="I4" s="6"/>
+      <c r="J4" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1903,27 +1917,27 @@
       <c r="C5" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="17" t="s">
+      <c r="H5" s="13"/>
+      <c r="I5" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -1933,27 +1947,27 @@
       <c r="C6" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H6" s="29"/>
-      <c r="I6" s="17" t="s">
+      <c r="H6" s="19"/>
+      <c r="I6" s="14" t="s">
         <v>106</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1963,79 +1977,79 @@
       <c r="C7" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="14" t="s">
         <v>106</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>108</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="6" t="s">
         <v>110</v>
       </c>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H9" s="27"/>
-      <c r="I9" s="17" t="s">
+      <c r="H9" s="19"/>
+      <c r="I9" s="14" t="s">
         <v>110</v>
       </c>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -2045,27 +2059,27 @@
       <c r="C10" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H10" s="29"/>
-      <c r="I10" s="21" t="s">
+      <c r="H10" s="19"/>
+      <c r="I10" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2075,35 +2089,35 @@
       <c r="C11" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>103</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="J11" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>117</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -2112,24 +2126,24 @@
       <c r="F12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="6" t="s">
         <v>98</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="I12" s="14" t="s">
         <v>100</v>
       </c>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>118</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -2138,16 +2152,15 @@
       <c r="F13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="17" t="s">
+      <c r="I13" s="14" t="s">
         <v>100</v>
       </c>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -2157,27 +2170,27 @@
       <c r="C14" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16" t="s">
+      <c r="H14" s="13"/>
+      <c r="I14" s="13" t="s">
         <v>105</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2187,29 +2200,29 @@
       <c r="C15" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I15" s="16" t="s">
+      <c r="I15" s="13" t="s">
         <v>105</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -2219,27 +2232,27 @@
       <c r="C16" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16" t="s">
+      <c r="H16" s="13"/>
+      <c r="I16" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="J16" s="11" t="s">
+      <c r="J16" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -2249,29 +2262,29 @@
       <c r="C17" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H17" s="21" t="s">
+      <c r="H17" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J17" s="11" t="s">
+      <c r="J17" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
@@ -2281,27 +2294,27 @@
       <c r="C18" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H18" s="16"/>
-      <c r="I18" s="21" t="s">
+      <c r="H18" s="13"/>
+      <c r="I18" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="J18" s="21" t="s">
+      <c r="J18" s="6" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
@@ -2311,29 +2324,29 @@
       <c r="C19" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H19" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="I19" s="17" t="s">
+      <c r="I19" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="J19" s="17" t="s">
+      <c r="J19" s="14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
@@ -2343,27 +2356,27 @@
       <c r="C20" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H20" s="8"/>
-      <c r="I20" s="17" t="s">
+      <c r="H20" s="1"/>
+      <c r="I20" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="J20" s="20" t="s">
+      <c r="J20" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
@@ -2373,153 +2386,152 @@
       <c r="C21" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H21" s="21" t="s">
+      <c r="H21" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I21" s="21" t="s">
+      <c r="I21" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="J21" s="23" t="s">
+      <c r="J21" s="16" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="H22" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I22" s="7" t="s">
+      <c r="I22" s="6" t="s">
         <v>109</v>
       </c>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G23" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H23" s="16"/>
-      <c r="I23" s="21" t="s">
+      <c r="H23" s="13"/>
+      <c r="I23" s="6" t="s">
         <v>109</v>
       </c>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F24" s="19" t="s">
+      <c r="F24" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G24" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="H24" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I24" s="17" t="s">
+      <c r="I24" s="14" t="s">
         <v>101</v>
       </c>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="19" t="s">
+      <c r="F25" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="H25" s="26"/>
-      <c r="I25" s="21" t="s">
+      <c r="I25" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="J25" s="19"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J25" s="13"/>
+    </row>
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G26" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="17" t="s">
+      <c r="H26" s="1"/>
+      <c r="I26" s="14" t="s">
         <v>127</v>
       </c>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
@@ -2529,16 +2541,16 @@
       <c r="C27" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="7" t="s">
         <v>123</v>
       </c>
       <c r="H27" s="1" t="s">
@@ -2547,7 +2559,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>12</v>
       </c>
@@ -2557,101 +2569,101 @@
       <c r="C28" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="G28" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="H28" s="17"/>
-      <c r="I28" s="16" t="s">
+      <c r="H28" s="14"/>
+      <c r="I28" s="13" t="s">
         <v>97</v>
       </c>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="E29" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F29" s="19" t="s">
+      <c r="F29" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="G29" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="H29" s="17" t="s">
+      <c r="H29" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="I29" s="16" t="s">
+      <c r="I29" s="13" t="s">
         <v>125</v>
       </c>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E30" s="19" t="s">
+      <c r="E30" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F30" s="19" t="s">
+      <c r="F30" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="G30" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="H30" s="25"/>
-      <c r="I30" s="16" t="s">
+      <c r="H30" s="18"/>
+      <c r="I30" s="13" t="s">
         <v>125</v>
       </c>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G31" s="7" t="s">
+      <c r="G31" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H31" s="17" t="s">
+      <c r="H31" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="I31" s="17" t="s">
+      <c r="I31" s="14" t="s">
         <v>127</v>
       </c>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>12</v>
       </c>
@@ -2661,25 +2673,25 @@
       <c r="C32" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E32" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="F32" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="G32" s="7" t="s">
         <v>123</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-    </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+    </row>
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>12</v>
       </c>
@@ -2689,43 +2701,43 @@
       <c r="C33" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="F33" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G33" s="10" t="s">
+      <c r="G33" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="H33" s="16"/>
-      <c r="I33" s="8" t="s">
+      <c r="H33" s="13"/>
+      <c r="I33" s="1" t="s">
         <v>97</v>
       </c>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E34" s="13" t="s">
+      <c r="E34" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F34" s="19" t="s">
+      <c r="F34" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G34" s="7" t="s">
+      <c r="G34" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="H34" s="17" t="s">
+      <c r="H34" s="14" t="s">
         <v>99</v>
       </c>
       <c r="I34" s="1" t="s">
@@ -2733,127 +2745,127 @@
       </c>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E35" s="13" t="s">
+      <c r="E35" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="19" t="s">
+      <c r="F35" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="7" t="s">
+      <c r="G35" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="H35" s="25"/>
-      <c r="I35" s="16" t="s">
+      <c r="H35" s="18"/>
+      <c r="I35" s="13" t="s">
         <v>102</v>
       </c>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E36" s="19" t="s">
+      <c r="E36" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F36" s="19" t="s">
+      <c r="F36" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G36" s="10" t="s">
+      <c r="G36" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="H36" s="28" t="s">
+      <c r="H36" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="I36" s="16"/>
+      <c r="I36" s="13"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F37" s="19" t="s">
+      <c r="F37" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G37" s="7" t="s">
+      <c r="G37" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="H37" s="25"/>
-      <c r="I37" s="16" t="s">
+      <c r="H37" s="18"/>
+      <c r="I37" s="13" t="s">
         <v>97</v>
       </c>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E38" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F38" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G38" s="10" t="s">
+      <c r="G38" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="H38" s="17" t="s">
+      <c r="H38" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="I38" s="8"/>
+      <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="E39" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="F39" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G39" s="10" t="s">
+      <c r="G39" s="7" t="s">
         <v>124</v>
       </c>
       <c r="H39" s="1"/>
-      <c r="I39" s="7" t="s">
+      <c r="I39" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J39" s="19"/>
-    </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="J39" s="13"/>
+    </row>
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>12</v>
       </c>
@@ -2863,29 +2875,29 @@
       <c r="C40" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D40" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E40" s="21" t="s">
+      <c r="E40" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F40" s="21" t="s">
+      <c r="F40" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="G40" s="7" t="s">
+      <c r="G40" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H40" s="17" t="s">
+      <c r="H40" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="I40" s="17" t="s">
+      <c r="I40" s="14" t="s">
         <v>107</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>12</v>
       </c>
@@ -2895,27 +2907,27 @@
       <c r="C41" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E41" s="21" t="s">
+      <c r="E41" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F41" s="21" t="s">
+      <c r="F41" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="G41" s="7" t="s">
+      <c r="G41" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H41" s="8"/>
-      <c r="I41" s="17" t="s">
+      <c r="H41" s="1"/>
+      <c r="I41" s="14" t="s">
         <v>107</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>12</v>
       </c>
@@ -2925,29 +2937,29 @@
       <c r="C42" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F42" s="7" t="s">
+      <c r="F42" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="G42" s="7" t="s">
+      <c r="G42" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I42" s="7" t="s">
+      <c r="I42" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="J42" s="11" t="s">
+      <c r="J42" s="8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>12</v>
       </c>
@@ -2957,246 +2969,487 @@
       <c r="C43" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E43" s="21" t="s">
+      <c r="E43" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F43" s="21" t="s">
+      <c r="F43" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="G43" s="21" t="s">
+      <c r="G43" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H43" s="16"/>
-      <c r="I43" s="21" t="s">
+      <c r="H43" s="13"/>
+      <c r="I43" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="J43" s="11" t="s">
+      <c r="J43" s="8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="11" t="s">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="12" t="s">
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="E44" s="13" t="s">
+      <c r="E44" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="F44" s="13" t="s">
+      <c r="F44" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="G44" s="10" t="s">
+      <c r="G44" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="H44" s="10" t="s">
+      <c r="H44" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="I44" s="13"/>
-      <c r="J44" s="11"/>
-    </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="11" t="s">
+      <c r="I44" s="10"/>
+      <c r="J44" s="8"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="12" t="s">
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E45" s="13" t="s">
+      <c r="E45" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="F45" s="13" t="s">
+      <c r="F45" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="G45" s="10" t="s">
+      <c r="G45" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="H45" s="10"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="11" t="s">
+      <c r="H45" s="7"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+    </row>
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="12" t="s">
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="E46" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="F46" s="10" t="s">
+      <c r="F46" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="G46" s="10" t="s">
+      <c r="G46" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="H46" s="10" t="s">
+      <c r="H46" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="I46" s="13"/>
-      <c r="J46" s="11"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="11" t="s">
+      <c r="I46" s="10"/>
+      <c r="J46" s="8"/>
+    </row>
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="12" t="s">
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E47" s="13" t="s">
+      <c r="E47" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="F47" s="13" t="s">
+      <c r="F47" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="G47" s="15" t="s">
+      <c r="G47" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="H47" s="14"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="14"/>
-    </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="11" t="s">
+      <c r="H47" s="11"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="11"/>
+    </row>
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="D48" s="12" t="s">
+      <c r="D48" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="E48" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="F48" s="10" t="s">
+      <c r="F48" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="G48" s="10" t="s">
+      <c r="G48" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="H48" s="11" t="s">
+      <c r="H48" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="I48" s="23" t="s">
+      <c r="I48" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="J48" s="23" t="s">
+      <c r="J48" s="16" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="11" t="s">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D49" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E49" s="20" t="s">
+      <c r="E49" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="F49" s="20" t="s">
+      <c r="F49" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="G49" s="10" t="s">
+      <c r="G49" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="H49" s="13"/>
-      <c r="I49" s="20" t="s">
+      <c r="H49" s="10"/>
+      <c r="I49" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="J49" s="20" t="s">
+      <c r="J49" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="11" t="s">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="D50" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="E50" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="F50" s="10" t="s">
+      <c r="F50" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="G50" s="10" t="s">
+      <c r="G50" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="H50" s="24" t="s">
+      <c r="H50" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="I50" s="23" t="s">
+      <c r="I50" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="J50" s="23" t="s">
+      <c r="J50" s="16" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="11" t="s">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="D51" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E51" s="23" t="s">
+      <c r="E51" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="F51" s="23" t="s">
+      <c r="F51" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="G51" s="10" t="s">
+      <c r="G51" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="H51" s="13"/>
-      <c r="I51" s="20" t="s">
+      <c r="H51" s="10"/>
+      <c r="I51" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="J51" s="20" t="s">
+      <c r="J51" s="7" t="s">
         <v>91</v>
       </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="F52" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="G52" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="H52" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="I52" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="J52" s="21"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B53" s="23"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="E53" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="F53" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="G53" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="H53" s="30"/>
+      <c r="I53" s="30"/>
+      <c r="J53" s="23"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E54" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="G54" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="H54" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="I54" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E55" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="G55" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="H55" s="30"/>
+      <c r="I55" s="30"/>
+      <c r="J55" s="13"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F56" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H56" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="I56" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="J56" s="1"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F57" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H57" s="18"/>
+      <c r="I57" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="J57" s="1"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="H58" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="I58" s="13"/>
+      <c r="J58" s="1"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E59" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F59" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H59" s="18"/>
+      <c r="I59" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="J59" s="1"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H60" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="I60" s="10"/>
+      <c r="J60" s="8"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H61" s="7"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3205,23 +3458,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
-    <col min="4" max="4" width="28.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="27.44140625" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3250,7 +3503,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3261,26 +3514,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT06A</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -3291,26 +3544,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT06A</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -3321,26 +3574,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT08A</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -3351,26 +3604,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT08A</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -3381,26 +3634,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT12A</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -3411,26 +3664,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT12A</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -3441,26 +3694,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT12A</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -3471,26 +3724,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT12A</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -3501,26 +3754,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT12A</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -3531,26 +3784,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT06A</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -3561,26 +3814,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT06A</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -3591,26 +3844,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT08A</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="I13" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -3621,26 +3874,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT08A</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I14" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -3651,26 +3904,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT08A</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" t="s">
         <v>87</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -3681,26 +3934,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT12A</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="H16" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="I16" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -3711,26 +3964,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT12A</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" t="s">
         <v>87</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="I17" s="7" t="s">
+      <c r="I17" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -3744,23 +3997,23 @@
       <c r="D18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E18" t="s">
         <v>88</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="H18" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="I18" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
@@ -3774,23 +4027,23 @@
       <c r="D19" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" t="s">
         <v>89</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H19" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="I19" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
@@ -3810,17 +4063,17 @@
       <c r="F20" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="H20" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="I20" s="7" t="s">
+      <c r="I20" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
@@ -3840,17 +4093,17 @@
       <c r="F21" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="H21" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="I21" s="7" t="s">
+      <c r="I21" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>18</v>
       </c>
@@ -3861,26 +4114,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT06A</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="H22" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="I22" s="7" t="s">
+      <c r="I22" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>18</v>
       </c>
@@ -3891,26 +4144,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT06A</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="H23" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I23" s="7" t="s">
+      <c r="I23" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>18</v>
       </c>
@@ -3921,26 +4174,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT08A</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="H24" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="I24" s="7" t="s">
+      <c r="I24" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
@@ -3951,26 +4204,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT08A</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="G25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="H25" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I25" s="7" t="s">
+      <c r="I25" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>18</v>
       </c>
@@ -3981,26 +4234,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT11A</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H26" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="I26" s="7" t="s">
+      <c r="I26" s="6" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>18</v>
       </c>
@@ -4011,26 +4264,26 @@
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT11A</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="G27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="H27" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="I27" s="7" t="s">
+      <c r="I27" s="6" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>18</v>
       </c>
@@ -4047,20 +4300,20 @@
       <c r="E28" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="G28" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H28" s="7" t="s">
+      <c r="H28" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="I28" s="7" t="s">
+      <c r="I28" s="6" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>18</v>
       </c>
@@ -4077,16 +4330,16 @@
       <c r="E29" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="G29" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H29" s="7" t="s">
+      <c r="H29" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="I29" s="7" t="s">
+      <c r="I29" s="6" t="s">
         <v>144</v>
       </c>
     </row>
@@ -4105,13 +4358,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -4119,7 +4372,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>81</v>
       </c>
@@ -4127,7 +4380,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -4135,7 +4388,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -4143,7 +4396,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -4151,7 +4404,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>85</v>
       </c>
@@ -4159,7 +4412,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>86</v>
       </c>
@@ -4167,7 +4420,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>87</v>
       </c>
@@ -4175,7 +4428,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>88</v>
       </c>
@@ -4183,7 +4436,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -4191,7 +4444,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -4199,7 +4452,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -4207,7 +4460,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>92</v>
       </c>
@@ -4215,7 +4468,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -4223,7 +4476,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -4231,7 +4484,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>95</v>
       </c>

</xml_diff>